<commit_message>
Add Detail Segment to Monitoring Donggala
</commit_message>
<xml_diff>
--- a/data/datek-cluster-donggala.xlsx
+++ b/data/datek-cluster-donggala.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A43770-4A6F-43E6-A849-1D82169F04CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84331992-98B3-49E5-918A-1CD79B05F321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -894,73 +894,73 @@
       <c r="B19" s="4"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="6:6" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Metro PAL1 & Switch DGL007
</commit_message>
<xml_diff>
--- a/data/datek-cluster-donggala.xlsx
+++ b/data/datek-cluster-donggala.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Repository\Telkom Projects\monitoring-site-premium-telegram-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84331992-98B3-49E5-918A-1CD79B05F321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1B8AC6-0CC6-4BE8-9955-34CD4E5CD05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>172.31.250.64</t>
   </si>
   <si>
-    <t>PGI</t>
-  </si>
-  <si>
     <t>ME-D7-PRG</t>
   </si>
   <si>
@@ -232,6 +229,30 @@
   </si>
   <si>
     <t>L2SW FH CITRANS</t>
+  </si>
+  <si>
+    <t>PAL1</t>
+  </si>
+  <si>
+    <t>ME9-D7-PAL1</t>
+  </si>
+  <si>
+    <t>172.31.250.96</t>
+  </si>
+  <si>
+    <t>DGL007</t>
+  </si>
+  <si>
+    <t>L2SW-D7-DGL007</t>
+  </si>
+  <si>
+    <t>10.199.162.2</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>PRG</t>
   </si>
 </sst>
 </file>
@@ -522,7 +543,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,16 +613,16 @@
     </row>
     <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
@@ -612,16 +633,16 @@
     </row>
     <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -632,159 +653,159 @@
     </row>
     <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="F8" s="5">
+        <v>12345</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="5">
-        <v>12345</v>
+        <v>23</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>62</v>
+        <v>33</v>
+      </c>
+      <c r="F11" s="5">
+        <v>12345</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="5">
         <v>12345</v>
@@ -792,19 +813,19 @@
     </row>
     <row r="14" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="5">
         <v>12345</v>
@@ -812,91 +833,123 @@
     </row>
     <row r="15" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="5">
-        <v>12345</v>
+        <v>10</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="D19" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="5">
         <v>12345</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="F19" s="5"/>
-    </row>
     <row r="20" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="F20" s="5"/>
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>

</xml_diff>